<commit_message>
Cartesian and Polar coordinates now fully functional, beginning to implement
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7EDB285-CCAE-4CE1-B382-9D69A60E6CCF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C9BA1651-59AB-45E9-88AA-DF436F22927D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Inputmanagement umgeschrieben</t>
+  </si>
+  <si>
+    <t>Polare Koordinaten ins Movement eingebaut</t>
+  </si>
+  <si>
+    <t>Movementverhalten weiter vertieft</t>
+  </si>
+  <si>
+    <t>3h</t>
   </si>
 </sst>
 </file>
@@ -392,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +522,28 @@
         <v>43397</v>
       </c>
     </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1">
+        <v>43399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Collision is somewhat alive now, still lots of work todo
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C9BA1651-59AB-45E9-88AA-DF436F22927D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0EB34FDA-D444-4337-B38E-2178B190B3F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>3h</t>
+  </si>
+  <si>
+    <t>Polarverhalten fertiggestellt und getested</t>
+  </si>
+  <si>
+    <t>Recherche von Collision detection</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +550,28 @@
         <v>43399</v>
       </c>
     </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1">
+        <v>43400</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>43400</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fuck collision response, now working on projectiles
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0EB34FDA-D444-4337-B38E-2178B190B3F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{023B88C5-F0E2-4A20-8306-8EE8ADFC317D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>Recherche von Collision detection</t>
+  </si>
+  <si>
+    <t>Mehr Arbeit an Kollision</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>Mehr Arbeit an Kollision…</t>
+  </si>
+  <si>
+    <t>10h</t>
   </si>
 </sst>
 </file>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F21"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,6 +584,28 @@
         <v>43400</v>
       </c>
     </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1">
+        <v>43401</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="1">
+        <v>43402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added some more dokumentation and ideas
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{023B88C5-F0E2-4A20-8306-8EE8ADFC317D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E26C591-A918-4081-A2CF-B3B2ED71E694}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>10h</t>
+  </si>
+  <si>
+    <t>Fazit: fick Kollision, ich mach was anderes</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +609,11 @@
         <v>43402</v>
       </c>
     </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Basic projectile functionality implemented, needs some more work
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E26C591-A918-4081-A2CF-B3B2ED71E694}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C73D5D0B-5877-49BE-B906-A3490724D1D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Fazit: fick Kollision, ich mach was anderes</t>
+  </si>
+  <si>
+    <t>Arbeit an der Architektur</t>
+  </si>
+  <si>
+    <t>Projektil Algorithmus</t>
+  </si>
+  <si>
+    <t>Spawnen von Projektilen und Grundstruktur steht</t>
   </si>
 </sst>
 </file>
@@ -422,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +623,39 @@
         <v>27</v>
       </c>
     </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="1">
+        <v>43403</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1">
+        <v>43403</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1">
+        <v>43403</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
forgot to save some stuff
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C73D5D0B-5877-49BE-B906-A3490724D1D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94D53AF8-ADF1-4D42-ACA8-39066DEFF155}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Spawnen von Projektilen und Grundstruktur steht</t>
+  </si>
+  <si>
+    <t>Architektur weiter ergänzt für bessere GC Optimierung</t>
+  </si>
+  <si>
+    <t>Funktionalität mit Timern implementiert (Projektilsystem)</t>
+  </si>
+  <si>
+    <t>Primitives Lebenssystem ist jetzt auch drinnen</t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F30"/>
+  <dimension ref="B2:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,6 +665,39 @@
         <v>43403</v>
       </c>
     </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1">
+        <v>43404</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43404</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1">
+        <v>43404</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
now starting to rework the ECS architecture, looks good so far
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94D53AF8-ADF1-4D42-ACA8-39066DEFF155}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2669065E-2F58-4633-9081-ABB2727851F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>Primitives Lebenssystem ist jetzt auch drinnen</t>
+  </si>
+  <si>
+    <t>Projektilsystem</t>
+  </si>
+  <si>
+    <t>Projektilsystem machte extreme Performance Probleme, versucht zu beheben (kein Erfolg)</t>
+  </si>
+  <si>
+    <t>Umbau der ECS Architektur aus Optimierungsgründen</t>
   </si>
 </sst>
 </file>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F34"/>
+  <dimension ref="B2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,6 +707,39 @@
         <v>43404</v>
       </c>
     </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="1">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="1">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="1">
+        <v>43405</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added basic menu functionality
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2669065E-2F58-4633-9081-ABB2727851F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CE9DD57B-2FAE-4C8A-A5FA-F918ADA86451}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Umbau der ECS Architektur aus Optimierungsgründen</t>
+  </si>
+  <si>
+    <t>Architektur umgebaut</t>
+  </si>
+  <si>
+    <t>Projektilsystem funktionsfähig</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F39"/>
+  <dimension ref="B2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +743,29 @@
         <v>15</v>
       </c>
       <c r="F39" s="1">
-        <v>43405</v>
+        <v>43406</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="1">
+        <v>43406</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1">
+        <v>43406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some work with Breunig
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E9317C0-AF82-4883-B350-C51A40599658}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4E2463DE-690E-41F1-9724-94D5A97F6F95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -28,36 +28,18 @@
     <t>Beschreibung</t>
   </si>
   <si>
-    <t>Dauer</t>
-  </si>
-  <si>
     <t>Debugging</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>Codeverwaltung</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>Beginn von Movementverhalten</t>
   </si>
   <si>
     <t>Beginn von Inputmanagement</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t>6h 30min</t>
-  </si>
-  <si>
-    <t>1h 30min</t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -67,9 +49,6 @@
     <t>Inputmanagement implementiert</t>
   </si>
   <si>
-    <t>5h</t>
-  </si>
-  <si>
     <t>Movementverhalten vertieft (noch inkorrekt)</t>
   </si>
   <si>
@@ -82,9 +61,6 @@
     <t>Movementverhalten weiter vertieft</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>Polarverhalten fertiggestellt und getested</t>
   </si>
   <si>
@@ -94,15 +70,9 @@
     <t>Mehr Arbeit an Kollision</t>
   </si>
   <si>
-    <t>8h</t>
-  </si>
-  <si>
     <t>Mehr Arbeit an Kollision…</t>
   </si>
   <si>
-    <t>10h</t>
-  </si>
-  <si>
     <t>Fazit: fick Kollision, ich mach was anderes</t>
   </si>
   <si>
@@ -146,6 +116,9 @@
   </si>
   <si>
     <t>Code gesäubert</t>
+  </si>
+  <si>
+    <t>Dauer in h</t>
   </si>
 </sst>
 </file>
@@ -466,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,73 +453,79 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>SUM(D4:D48)</f>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
+      <c r="D4">
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="F10" s="1">
         <v>43396</v>
@@ -554,10 +533,10 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
       </c>
       <c r="F11" s="1">
         <v>43396</v>
@@ -565,10 +544,10 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
       </c>
       <c r="F12" s="1">
         <v>43396</v>
@@ -576,10 +555,10 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>43397</v>
@@ -587,10 +566,10 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
       </c>
       <c r="F16" s="1">
         <v>43398</v>
@@ -598,10 +577,10 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
       </c>
       <c r="F18" s="1">
         <v>43399</v>
@@ -609,10 +588,10 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
       </c>
       <c r="F20" s="1">
         <v>43400</v>
@@ -620,10 +599,10 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
       </c>
       <c r="F21" s="1">
         <v>43400</v>
@@ -631,10 +610,10 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
       </c>
       <c r="F23" s="1">
         <v>43401</v>
@@ -642,10 +621,10 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
       </c>
       <c r="F25" s="1">
         <v>43402</v>
@@ -653,15 +632,15 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
       </c>
       <c r="F28" s="1">
         <v>43403</v>
@@ -669,10 +648,10 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
       </c>
       <c r="F29" s="1">
         <v>43403</v>
@@ -680,10 +659,10 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
         <v>20</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
       </c>
       <c r="F30" s="1">
         <v>43403</v>
@@ -691,10 +670,10 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="F32" s="1">
         <v>43404</v>
@@ -702,10 +681,10 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
       </c>
       <c r="F33" s="1">
         <v>43404</v>
@@ -713,10 +692,10 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="F34" s="1">
         <v>43404</v>
@@ -724,10 +703,10 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
       </c>
       <c r="F36" s="1">
         <v>43405</v>
@@ -735,10 +714,10 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
       </c>
       <c r="F37" s="1">
         <v>43405</v>
@@ -746,10 +725,10 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
       </c>
       <c r="F39" s="1">
         <v>43406</v>
@@ -757,10 +736,10 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
       </c>
       <c r="F41" s="1">
         <v>43406</v>
@@ -768,10 +747,10 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
       </c>
       <c r="F42" s="1">
         <v>43406</v>
@@ -779,10 +758,10 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
       </c>
       <c r="F44" s="1">
         <v>43407</v>
@@ -790,10 +769,10 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
       </c>
       <c r="F46" s="1">
         <v>43408</v>
@@ -801,10 +780,10 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
       </c>
       <c r="F48" s="1">
         <v>43409</v>

</xml_diff>

<commit_message>
fixed the Timers and found the collision problem, will fix it tomorrow
</commit_message>
<xml_diff>
--- a/Doku/Frackiewicz Zeitaufwand.xlsx
+++ b/Doku/Frackiewicz Zeitaufwand.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4E2463DE-690E-41F1-9724-94D5A97F6F95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DD2CADE6-6065-42BD-A4EA-A7DC712E97FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Implementierung von ECS</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>Dauer in h</t>
+  </si>
+  <si>
+    <t>6-7-8-Nov</t>
+  </si>
+  <si>
+    <t>Menu verbessert und kleine Verschönerungen im Code</t>
+  </si>
+  <si>
+    <t>Erweiterung des Kollisionssystem mit Swept AABB</t>
   </si>
 </sst>
 </file>
@@ -437,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F48"/>
+  <dimension ref="B2:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,6 +798,28 @@
         <v>43409</v>
       </c>
     </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="F52" s="1">
+        <v>43413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>